<commit_message>
finish BLAST on 16S .xlsx, added to assign taxconomy ref db
</commit_message>
<xml_diff>
--- a/WADE003-arcticpred_dada2_QAQC_16SP1+2.Rdata.xlsx
+++ b/WADE003-arcticpred_dada2_QAQC_16SP1+2.Rdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE892F5F-F819-4BB0-A3EA-D3F73A48336A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{BE892F5F-F819-4BB0-A3EA-D3F73A48336A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A04D0154-B9DE-44B4-8D07-A1164725A11E}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="222">
   <si>
     <t>rownames</t>
   </si>
@@ -674,13 +674,25 @@
   </si>
   <si>
     <t xml:space="preserve">Leptoclinus maculatus &amp; Lumpenus fabricii  </t>
+  </si>
+  <si>
+    <t>Myoxocephalus quadricornis</t>
+  </si>
+  <si>
+    <t>Pungitius pungitius</t>
+  </si>
+  <si>
+    <t>&gt;99% Oncorhynchus tshawytscha AND Oncorhynchus kisutch</t>
+  </si>
+  <si>
+    <t>nothing &gt;98%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,8 +721,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,6 +749,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -733,10 +769,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -744,8 +782,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1050,25 +1092,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J105" sqref="J105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.46484375" customWidth="1"/>
-    <col min="2" max="2" width="10.86328125" customWidth="1"/>
-    <col min="3" max="3" width="12.1328125" customWidth="1"/>
-    <col min="4" max="4" width="12.86328125" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1103,7 +1145,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1135,7 +1177,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1167,7 +1209,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1199,7 +1241,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1231,7 +1273,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1263,7 +1305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1295,7 +1337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1327,7 +1369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1338,7 +1380,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1402,7 +1444,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1434,7 +1476,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1466,7 +1508,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1486,7 +1528,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1518,7 +1560,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1550,7 +1592,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1582,7 +1624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1614,7 +1656,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -1640,7 +1682,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1669,7 +1711,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1677,7 +1719,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1709,7 +1751,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1741,7 +1783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>69</v>
       </c>
@@ -1758,7 +1800,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -1784,7 +1826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1816,7 +1858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -1845,7 +1887,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -1874,7 +1916,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1906,7 +1948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -1935,7 +1977,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -1964,7 +2006,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -1984,7 +2026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2013,7 +2055,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -2042,7 +2084,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2071,7 +2113,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2100,7 +2142,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -2120,7 +2162,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>86</v>
       </c>
@@ -2134,7 +2176,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -2151,7 +2193,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -2171,7 +2213,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -2203,7 +2245,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -2235,7 +2277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>99</v>
       </c>
@@ -2264,7 +2306,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>100</v>
       </c>
@@ -2284,7 +2326,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -2313,7 +2355,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -2342,7 +2384,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -2371,7 +2413,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2400,7 +2442,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -2429,15 +2471,18 @@
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="50" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B50" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -2462,8 +2507,11 @@
       <c r="H51" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K51" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>109</v>
       </c>
@@ -2488,8 +2536,11 @@
       <c r="H52" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K52" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -2521,33 +2572,36 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="54" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B54" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="B54" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K54" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>115</v>
       </c>
@@ -2579,7 +2633,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -2604,8 +2658,11 @@
       <c r="H56" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K56" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -2637,7 +2694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -2669,30 +2726,33 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B59" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="B59" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K59" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -2724,33 +2784,33 @@
         <v>126</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+    <row r="61" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B61" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="B61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>128</v>
       </c>
@@ -2770,7 +2830,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>131</v>
       </c>
@@ -2795,8 +2855,11 @@
       <c r="H63" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K63" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>132</v>
       </c>
@@ -2810,7 +2873,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -2830,7 +2893,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>137</v>
       </c>
@@ -2862,7 +2925,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -2894,7 +2957,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>143</v>
       </c>
@@ -2926,21 +2989,24 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+    <row r="69" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B69" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>150</v>
       </c>
@@ -2972,7 +3038,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>153</v>
       </c>
@@ -3004,7 +3070,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>156</v>
       </c>
@@ -3036,7 +3102,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>160</v>
       </c>
@@ -3068,7 +3134,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>165</v>
       </c>
@@ -3100,7 +3166,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>170</v>
       </c>
@@ -3125,8 +3191,11 @@
       <c r="H75" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K75" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -3158,7 +3227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>172</v>
       </c>
@@ -3190,56 +3259,62 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
+    <row r="78" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B78" t="s">
-        <v>11</v>
-      </c>
-      <c r="C78" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" t="s">
-        <v>13</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="B78" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H78" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
+      <c r="K78" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B79" t="s">
-        <v>11</v>
-      </c>
-      <c r="C79" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" t="s">
-        <v>13</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="B79" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K79" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>176</v>
       </c>
@@ -3271,7 +3346,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>179</v>
       </c>
@@ -3303,7 +3378,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>180</v>
       </c>
@@ -3335,7 +3410,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>181</v>
       </c>
@@ -3367,7 +3442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>182</v>
       </c>
@@ -3387,7 +3462,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>183</v>
       </c>
@@ -3419,7 +3494,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>184</v>
       </c>
@@ -3451,7 +3526,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>185</v>
       </c>
@@ -3470,8 +3545,11 @@
       <c r="F87" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K87" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>186</v>
       </c>
@@ -3497,7 +3575,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>187</v>
       </c>
@@ -3529,7 +3607,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>188</v>
       </c>
@@ -3561,7 +3639,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>189</v>
       </c>
@@ -3587,7 +3665,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>190</v>
       </c>
@@ -3619,7 +3697,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>191</v>
       </c>
@@ -3651,7 +3729,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>192</v>
       </c>
@@ -3670,8 +3748,11 @@
       <c r="F94" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K94" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>193</v>
       </c>
@@ -3703,12 +3784,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>195</v>
       </c>
@@ -3734,7 +3815,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>196</v>
       </c>
@@ -3766,7 +3847,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>197</v>
       </c>
@@ -3798,7 +3879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>198</v>
       </c>
@@ -3824,7 +3905,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>199</v>
       </c>
@@ -3856,7 +3937,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -3888,7 +3969,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>201</v>
       </c>
@@ -3920,7 +4001,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>209</v>
       </c>
@@ -3949,7 +4030,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>210</v>
       </c>
@@ -3981,7 +4062,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>211</v>
       </c>

</xml_diff>